<commit_message>
Update to Player Keys
</commit_message>
<xml_diff>
--- a/PlayerKeys.xlsx
+++ b/PlayerKeys.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I136"/>
+  <dimension ref="A1:I144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5475,6 +5475,302 @@
         <v>32675</v>
       </c>
     </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>espino</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>paolo</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>502179</v>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>espip001</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>espinpa01</t>
+        </is>
+      </c>
+      <c r="F137" t="n">
+        <v>8246</v>
+      </c>
+      <c r="G137" t="n">
+        <v>2017</v>
+      </c>
+      <c r="H137" t="n">
+        <v>2021</v>
+      </c>
+      <c r="I137" t="n">
+        <v>29989</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>stroman</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>marcus</t>
+        </is>
+      </c>
+      <c r="C138" t="n">
+        <v>573186</v>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>strom001</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>stromma01</t>
+        </is>
+      </c>
+      <c r="F138" t="n">
+        <v>13431</v>
+      </c>
+      <c r="G138" t="n">
+        <v>2014</v>
+      </c>
+      <c r="H138" t="n">
+        <v>2021</v>
+      </c>
+      <c r="I138" t="n">
+        <v>32815</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>pineda</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>michael</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>501381</v>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>pinem001</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>pinedmi01</t>
+        </is>
+      </c>
+      <c r="F139" t="n">
+        <v>5372</v>
+      </c>
+      <c r="G139" t="n">
+        <v>2011</v>
+      </c>
+      <c r="H139" t="n">
+        <v>2021</v>
+      </c>
+      <c r="I139" t="n">
+        <v>30937</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>foltynewicz</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>mike</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>592314</v>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>foltm001</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>foltymi01</t>
+        </is>
+      </c>
+      <c r="F140" t="n">
+        <v>10811</v>
+      </c>
+      <c r="G140" t="n">
+        <v>2014</v>
+      </c>
+      <c r="H140" t="n">
+        <v>2021</v>
+      </c>
+      <c r="I140" t="n">
+        <v>31819</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>garcia</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>luis</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>671277</v>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>garcl006</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>garcilu04</t>
+        </is>
+      </c>
+      <c r="F141" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G141" t="n">
+        <v>2020</v>
+      </c>
+      <c r="H141" t="n">
+        <v>2021</v>
+      </c>
+      <c r="I141" t="n">
+        <v>4684365</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>ohtani</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>shohei</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>660271</v>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>ohtas001</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>ohtansh01</t>
+        </is>
+      </c>
+      <c r="F142" t="n">
+        <v>19755</v>
+      </c>
+      <c r="G142" t="n">
+        <v>2018</v>
+      </c>
+      <c r="H142" t="n">
+        <v>2021</v>
+      </c>
+      <c r="I142" t="n">
+        <v>39832</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>smith</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>caleb</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>592761</v>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>smitc006</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>smithca03</t>
+        </is>
+      </c>
+      <c r="F143" t="n">
+        <v>14875</v>
+      </c>
+      <c r="G143" t="n">
+        <v>2017</v>
+      </c>
+      <c r="H143" t="n">
+        <v>2021</v>
+      </c>
+      <c r="I143" t="n">
+        <v>36081</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>pivetta</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>nick</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>601713</v>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>piven001</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>pivetni01</t>
+        </is>
+      </c>
+      <c r="F144" t="n">
+        <v>15454</v>
+      </c>
+      <c r="G144" t="n">
+        <v>2017</v>
+      </c>
+      <c r="H144" t="n">
+        <v>2021</v>
+      </c>
+      <c r="I144" t="n">
+        <v>36071</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fangraphs ID Lookups for Hitters
</commit_message>
<xml_diff>
--- a/PlayerKeys.xlsx
+++ b/PlayerKeys.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I144"/>
+  <dimension ref="A1:I145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5771,6 +5771,41 @@
         <v>36071</v>
       </c>
     </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>soto</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>juan</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>665742</v>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>sotoj001</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>sotoju01</t>
+        </is>
+      </c>
+      <c r="F145" t="n">
+        <v>20123</v>
+      </c>
+      <c r="G145" t="n">
+        <v>2018</v>
+      </c>
+      <c r="H145" t="n">
+        <v>2021</v>
+      </c>
+      <c r="I145" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added manual Method for names that cause an error
</commit_message>
<xml_diff>
--- a/PlayerKeys.xlsx
+++ b/PlayerKeys.xlsx
@@ -1,29 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke DeSando\Documents\Git\Beat-The-Streak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF4017E-C8C6-4D6D-A420-65068B0EEB56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C8CF52-3FF2-4F6C-A6EA-2266F0E53851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$1021</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4089" uniqueCount="3340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4129" uniqueCount="3352">
   <si>
     <t>name_last</t>
   </si>
@@ -10043,6 +10040,42 @@
   </si>
   <si>
     <t>dobnara01</t>
+  </si>
+  <si>
+    <t>howas003</t>
+  </si>
+  <si>
+    <t>howarsp01</t>
+  </si>
+  <si>
+    <t>lynch</t>
+  </si>
+  <si>
+    <t>lyncd001</t>
+  </si>
+  <si>
+    <t>lynchda02</t>
+  </si>
+  <si>
+    <t>jax</t>
+  </si>
+  <si>
+    <t>jax-g001</t>
+  </si>
+  <si>
+    <t>jaxgr01</t>
+  </si>
+  <si>
+    <t>j. c.</t>
+  </si>
+  <si>
+    <t>mejiaje02</t>
+  </si>
+  <si>
+    <t>mejij002</t>
+  </si>
+  <si>
+    <t>j.a.</t>
   </si>
 </sst>
 </file>
@@ -10405,17 +10438,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1021"/>
+  <dimension ref="A1:I1031"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="B244" sqref="B244"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1007" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1032" sqref="A1032"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -37057,7 +37087,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="1009" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1009" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1009" t="s">
         <v>3297</v>
       </c>
@@ -37083,7 +37113,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="1010" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1010" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1010" t="s">
         <v>3300</v>
       </c>
@@ -37109,7 +37139,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="1011" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1011" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1011" t="s">
         <v>3304</v>
       </c>
@@ -37135,7 +37165,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="1012" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1012" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1012" t="s">
         <v>3307</v>
       </c>
@@ -37161,7 +37191,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="1013" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1013" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1013" t="s">
         <v>3310</v>
       </c>
@@ -37187,7 +37217,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="1014" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1014" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1014" t="s">
         <v>3314</v>
       </c>
@@ -37213,7 +37243,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="1015" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1015" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1015" t="s">
         <v>3317</v>
       </c>
@@ -37239,7 +37269,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="1016" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1016" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1016" t="s">
         <v>1561</v>
       </c>
@@ -37265,7 +37295,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="1017" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1017" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1017" t="s">
         <v>3323</v>
       </c>
@@ -37291,7 +37321,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="1018" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1018" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1018" t="s">
         <v>3327</v>
       </c>
@@ -37317,7 +37347,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="1019" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1019" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1019" t="s">
         <v>3330</v>
       </c>
@@ -37343,7 +37373,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="1020" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1020" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1020" t="s">
         <v>3333</v>
       </c>
@@ -37369,7 +37399,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="1021" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1021" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1021" t="s">
         <v>3337</v>
       </c>
@@ -37395,8 +37425,297 @@
         <v>2021</v>
       </c>
     </row>
+    <row r="1022" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1022" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1022" t="s">
+        <v>2195</v>
+      </c>
+      <c r="C1022">
+        <v>502624</v>
+      </c>
+      <c r="D1022" t="s">
+        <v>2388</v>
+      </c>
+      <c r="E1022" t="s">
+        <v>2389</v>
+      </c>
+      <c r="F1022">
+        <v>6895</v>
+      </c>
+      <c r="G1022">
+        <v>2014</v>
+      </c>
+      <c r="H1022">
+        <v>2021</v>
+      </c>
+      <c r="I1022">
+        <v>32690</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1023" t="s">
+        <v>2014</v>
+      </c>
+      <c r="B1023" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1023">
+        <v>605164</v>
+      </c>
+      <c r="D1023" t="s">
+        <v>2015</v>
+      </c>
+      <c r="E1023" t="s">
+        <v>2016</v>
+      </c>
+      <c r="F1023">
+        <v>12917</v>
+      </c>
+      <c r="G1023">
+        <v>2012</v>
+      </c>
+      <c r="H1023">
+        <v>2021</v>
+      </c>
+      <c r="I1023">
+        <v>32094</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1024" t="s">
+        <v>3053</v>
+      </c>
+      <c r="B1024" t="s">
+        <v>2648</v>
+      </c>
+      <c r="C1024">
+        <v>675921</v>
+      </c>
+      <c r="D1024" t="s">
+        <v>3340</v>
+      </c>
+      <c r="E1024" t="s">
+        <v>3341</v>
+      </c>
+      <c r="F1024">
+        <v>-1</v>
+      </c>
+      <c r="G1024">
+        <v>2020</v>
+      </c>
+      <c r="H1024">
+        <v>2021</v>
+      </c>
+      <c r="I1024">
+        <v>41072</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1025" t="s">
+        <v>2111</v>
+      </c>
+      <c r="B1025" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1025">
+        <v>453562</v>
+      </c>
+      <c r="D1025" t="s">
+        <v>2112</v>
+      </c>
+      <c r="E1025" t="s">
+        <v>2113</v>
+      </c>
+      <c r="F1025">
+        <v>4153</v>
+      </c>
+      <c r="G1025">
+        <v>2010</v>
+      </c>
+      <c r="H1025">
+        <v>2021</v>
+      </c>
+      <c r="I1025">
+        <v>30145</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1026" t="s">
+        <v>309</v>
+      </c>
+      <c r="B1026" t="s">
+        <v>290</v>
+      </c>
+      <c r="C1026">
+        <v>605452</v>
+      </c>
+      <c r="D1026" t="s">
+        <v>1960</v>
+      </c>
+      <c r="E1026" t="s">
+        <v>1961</v>
+      </c>
+      <c r="F1026">
+        <v>12972</v>
+      </c>
+      <c r="G1026">
+        <v>2015</v>
+      </c>
+      <c r="H1026">
+        <v>2021</v>
+      </c>
+      <c r="I1026">
+        <v>32684</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1027" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1027" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1027">
+        <v>542881</v>
+      </c>
+      <c r="D1027" t="s">
+        <v>2171</v>
+      </c>
+      <c r="E1027" t="s">
+        <v>2172</v>
+      </c>
+      <c r="F1027">
+        <v>12880</v>
+      </c>
+      <c r="G1027">
+        <v>2016</v>
+      </c>
+      <c r="H1027">
+        <v>2021</v>
+      </c>
+      <c r="I1027">
+        <v>32151</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1028" t="s">
+        <v>3342</v>
+      </c>
+      <c r="B1028" t="s">
+        <v>1806</v>
+      </c>
+      <c r="C1028">
+        <v>663738</v>
+      </c>
+      <c r="D1028" t="s">
+        <v>3343</v>
+      </c>
+      <c r="E1028" t="s">
+        <v>3344</v>
+      </c>
+      <c r="F1028">
+        <v>-1</v>
+      </c>
+      <c r="G1028">
+        <v>2021</v>
+      </c>
+      <c r="H1028">
+        <v>2021</v>
+      </c>
+      <c r="I1028">
+        <v>41227</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1029" t="s">
+        <v>3345</v>
+      </c>
+      <c r="B1029" t="s">
+        <v>3301</v>
+      </c>
+      <c r="C1029">
+        <v>643377</v>
+      </c>
+      <c r="D1029" t="s">
+        <v>3346</v>
+      </c>
+      <c r="E1029" t="s">
+        <v>3347</v>
+      </c>
+      <c r="F1029">
+        <v>-1</v>
+      </c>
+      <c r="G1029">
+        <v>2021</v>
+      </c>
+      <c r="H1029">
+        <v>2021</v>
+      </c>
+      <c r="I1029">
+        <v>42604</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1030" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B1030" t="s">
+        <v>3348</v>
+      </c>
+      <c r="C1030">
+        <v>650496</v>
+      </c>
+      <c r="D1030" t="s">
+        <v>3350</v>
+      </c>
+      <c r="E1030" t="s">
+        <v>3349</v>
+      </c>
+      <c r="F1030">
+        <v>-1</v>
+      </c>
+      <c r="G1030">
+        <v>2021</v>
+      </c>
+      <c r="H1030">
+        <v>2021</v>
+      </c>
+      <c r="I1030">
+        <v>40421</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1031" t="s">
+        <v>1736</v>
+      </c>
+      <c r="B1031" t="s">
+        <v>3351</v>
+      </c>
+      <c r="C1031">
+        <v>457918</v>
+      </c>
+      <c r="D1031" t="s">
+        <v>2412</v>
+      </c>
+      <c r="E1031" t="s">
+        <v>2413</v>
+      </c>
+      <c r="F1031">
+        <v>7410</v>
+      </c>
+      <c r="G1031">
+        <v>2007</v>
+      </c>
+      <c r="H1031">
+        <v>2021</v>
+      </c>
+      <c r="I1031">
+        <v>28817</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I1021" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>